<commit_message>
accounting for labor day
</commit_message>
<xml_diff>
--- a/_data/Syllabus.xlsx
+++ b/_data/Syllabus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg.ryslik/personalRepos/OSU/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E4A100-F62B-8543-A41E-40FDC4D573B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FBD560-FFCC-CE44-9056-497383A42E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-74020" yWindow="-11480" windowWidth="47500" windowHeight="24500" xr2:uid="{DE38FA10-6465-D545-92BA-8AB89C1CB985}"/>
   </bookViews>
@@ -1054,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1F1D59-BDDB-1F49-AD29-AEA302336D29}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,7 +1069,7 @@
     <col min="8" max="8" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1138,13 +1138,10 @@
         <v>Mon</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1161,11 +1158,11 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="L4">
-        <v>191958</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1182,14 +1179,8 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1204,10 +1195,16 @@
         <v>Wed</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1224,14 +1221,8 @@
       <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1248,11 +1239,14 @@
       <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1269,14 +1263,11 @@
       <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1291,10 +1282,16 @@
         <v>Wed</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1310,10 +1307,10 @@
         <v>Mon</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1329,16 +1326,10 @@
         <v>Wed</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1356,8 +1347,14 @@
       <c r="E13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1375,11 +1372,8 @@
       <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1395,13 +1389,13 @@
         <v>Mon</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1417,7 +1411,10 @@
         <v>Wed</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1438,12 +1435,6 @@
       <c r="E17" t="s">
         <v>21</v>
       </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1463,6 +1454,12 @@
       <c r="E18" t="s">
         <v>21</v>
       </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1499,13 +1496,7 @@
         <v>Wed</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1525,6 +1516,12 @@
       </c>
       <c r="E21" t="s">
         <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>